<commit_message>
ported I2C master driver
</commit_message>
<xml_diff>
--- a/rev_b/sfw/U1001_Firmware/Microcontroller_Peripheral_Map.xlsx
+++ b/rev_b/sfw/U1001_Firmware/Microcontroller_Peripheral_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewm\OneDrive\Documents\KiCad Projects\Projects\Nixie_Clock\rev_b\sfw\U1001_Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAB4A9B-EE24-4B07-AFB9-B5098835F34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEA95D-636B-4450-BBAC-FB10650FF0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B7D91EF5-14DE-4003-8C97-5F77E28EC198}"/>
   </bookViews>
@@ -551,7 +551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3552A37-77FD-49A8-A79A-02C6EC063803}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>